<commit_message>
calculate IX velocity from flowrate
</commit_message>
<xml_diff>
--- a/Shiny-GAC/GAC_config.xlsx
+++ b/Shiny-GAC/GAC_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/colantonio_david_epa_gov/Documents/Profile/Documents/GitHub/Water_Treatment_Models/Shiny-GAC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/burkhardt_jonathan_epa_gov/Documents/Profile/Desktop/Git/Water_Treatment_Models/Shiny-GAC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A87A5872-C296-4B94-BBA8-0CC8B564D099}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBE5B243-B9EB-422F-97FE-6AEEC7EB469C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="7" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
+    <workbookView xWindow="58740" yWindow="10755" windowWidth="19065" windowHeight="15015" firstSheet="2" activeTab="3" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -304,6 +304,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,14 +322,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -366,7 +363,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -472,7 +469,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -614,7 +611,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -926,15 +923,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401BCFB4-DB77-4CE9-BB3A-E676947AF423}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -945,7 +942,7 @@
       <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D1" t="s">
@@ -959,7 +956,7 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="11">
         <v>50000</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -973,7 +970,7 @@
       <c r="B3">
         <v>174</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>50000</v>
       </c>
       <c r="D3" t="s">
@@ -987,7 +984,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="11">
         <v>0</v>
       </c>
       <c r="D4" t="s">
@@ -1001,7 +998,7 @@
       <c r="B5">
         <v>174</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="11">
         <v>0</v>
       </c>
       <c r="D5" t="s">
@@ -1621,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C024A4-1F50-44C3-AF99-7D9007347445}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1643,61 +1640,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3E377063FFE5489A04E78E6AF321F7" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d56b0910c09b2f28088e837fc8a4b1f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns4="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns6="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xmlns:ns7="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c38d2d5698dbedce593845e142ad0a0f" ns1:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2154,23 +2096,85 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D265CA-67CD-4AD3-99A3-30810910E78A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
+    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2191,25 +2195,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D265CA-67CD-4AD3-99A3-30810910E78A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
-    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>